<commit_message>
Tooling comments improved.  Mapping typos fixed.  Atefacts regenerated.  Typos resoved.
</commit_message>
<xml_diff>
--- a/mappings/land-cmip5-to-cmip6-mappings.xlsx
+++ b/mappings/land-cmip5-to-cmip6-mappings.xlsx
@@ -1,16 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="true"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <workbookPr date1904="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macg/dev/esdoc/repos/cmip6/cmip6-specializations-land/mappings/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -122,9 +134,6 @@
     <t>Permafrost &gt; List Of Gases</t>
   </si>
   <si>
-    <t>cmip6.land.carbon_cycle.permafrost_carbon.Emitted_greenhouse_gases</t>
-  </si>
-  <si>
     <t>Soil &gt; List Of Carbon Pools</t>
   </si>
   <si>
@@ -504,17 +513,16 @@
   </si>
   <si>
     <t>cmip6.land.vegetation.vegetation_types</t>
+  </si>
+  <si>
+    <t>cmip6.land.carbon_cycle.permafrost_carbon.emitted_greenhouse_gases</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -522,22 +530,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="18"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -550,7 +543,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -572,104 +565,348 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
-    <pageSetUpPr fitToPage="true"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor rgb="FFFFFFFF"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:C109"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C52" activeCellId="0" sqref="C52"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="50.4336734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="52.3316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="62.8316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.33163265306122"/>
+    <col min="1" max="1" width="44.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3" s="3" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -680,7 +917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -689,7 +926,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -698,16 +935,16 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C4"/>
+    </row>
+    <row r="5" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -716,16 +953,16 @@
       </c>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C6"/>
+    </row>
+    <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -734,18 +971,18 @@
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
@@ -754,16 +991,16 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C10"/>
+    </row>
+    <row r="11" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
@@ -772,32 +1009,32 @@
       </c>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C12"/>
+    </row>
+    <row r="13" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
@@ -808,7 +1045,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
@@ -817,7 +1054,7 @@
       </c>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
@@ -828,7 +1065,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
@@ -839,7 +1076,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
@@ -850,7 +1087,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
@@ -861,7 +1098,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
         <v>18</v>
       </c>
@@ -870,7 +1107,7 @@
       </c>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
         <v>18</v>
       </c>
@@ -879,12 +1116,12 @@
       </c>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
         <v>32</v>
       </c>
@@ -893,7 +1130,7 @@
       </c>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>32</v>
       </c>
@@ -901,837 +1138,835 @@
         <v>34</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="27" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="0"/>
-    </row>
-    <row r="28" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>37</v>
+      </c>
+      <c r="C27"/>
+    </row>
+    <row r="28" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="29" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="5" t="s">
+    </row>
+    <row r="33" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="5" t="s">
+      <c r="C33" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="5" t="s">
+    </row>
+    <row r="34" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B34" s="5" t="s">
+      <c r="C34" s="5"/>
+    </row>
+    <row r="35" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="5"/>
-    </row>
-    <row r="35" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="5" t="s">
+      <c r="C35" s="5"/>
+    </row>
+    <row r="36" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="5"/>
-    </row>
-    <row r="36" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36" s="5" t="s">
+      <c r="C36" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="5" t="s">
+    </row>
+    <row r="37" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="5" t="s">
+      <c r="C37" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="5" t="s">
+    </row>
+    <row r="38" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B38" s="5" t="s">
+      <c r="C38" s="5"/>
+    </row>
+    <row r="39" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="5"/>
-    </row>
-    <row r="39" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="C39" s="5"/>
     </row>
-    <row r="40" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
     </row>
-    <row r="41" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="C41" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="5" t="s">
+    </row>
+    <row r="42" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B42" s="5" t="s">
+      <c r="C42" s="5"/>
+    </row>
+    <row r="43" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C42" s="5"/>
-    </row>
-    <row r="43" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B43" s="5" t="s">
+      <c r="C43" s="5"/>
+    </row>
+    <row r="44" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="5"/>
-    </row>
-    <row r="44" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B44" s="5" t="s">
+      <c r="C44" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C44" s="5" t="s">
+    </row>
+    <row r="45" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B45" s="5" t="s">
+      <c r="C45" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="46" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C46" s="5"/>
     </row>
-    <row r="47" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C47" s="5"/>
     </row>
-    <row r="48" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
     </row>
-    <row r="49" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="C49" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C49" s="5" t="s">
+    </row>
+    <row r="50" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B50" s="5" t="s">
+      <c r="C50" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C50" s="5" t="s">
+    </row>
+    <row r="51" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B51" s="5" t="s">
+      <c r="C51" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C51" s="5" t="s">
+    </row>
+    <row r="52" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B52" s="5" t="s">
+      <c r="C52" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C52" s="5" t="s">
+    </row>
+    <row r="53" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" s="5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B53" s="5" t="s">
+      <c r="C53" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C53" s="5" t="s">
+    </row>
+    <row r="54" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B54" s="5" t="s">
+      <c r="C54" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C54" s="5" t="s">
+    </row>
+    <row r="55" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B55" s="5" t="s">
+      <c r="C55" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="56" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="4"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
     </row>
-    <row r="57" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C57" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="58" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B58" s="5" t="s">
+      <c r="C58" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C58" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="59" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C59" s="5"/>
     </row>
-    <row r="60" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B60" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C60" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C60" s="5" t="s">
+    </row>
+    <row r="61" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A61" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="61" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B61" s="5" t="s">
+      <c r="C61" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C61" s="5" t="s">
+    </row>
+    <row r="62" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="62" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B62" s="5" t="s">
+      <c r="C62" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C62" s="5" t="s">
+    </row>
+    <row r="63" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="63" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B63" s="5" t="s">
+      <c r="C63" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C63" s="5" t="s">
+    </row>
+    <row r="64" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="64" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>93</v>
-      </c>
       <c r="C64" s="5"/>
     </row>
-    <row r="65" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C65" s="5"/>
     </row>
-    <row r="66" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B66" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C66" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C66" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="67" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="4"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
     </row>
-    <row r="68" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B68" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="C68" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C68" s="5" t="s">
+    </row>
+    <row r="69" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A69" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C69" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C69" s="5" t="s">
+    <row r="70" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A70" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B70" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="70" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B70" s="5" t="s">
+      <c r="C70" s="5"/>
+    </row>
+    <row r="71" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A71" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B71" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="C70" s="5"/>
-    </row>
-    <row r="71" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B72" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C72" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C72" s="5" t="s">
+    </row>
+    <row r="73" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A73" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B73" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="73" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B73" s="5" t="s">
+      <c r="C73" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C73" s="5" t="s">
+    </row>
+    <row r="74" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A74" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B74" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="74" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B74" s="5" t="s">
+      <c r="C74" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C74" s="5" t="s">
+    </row>
+    <row r="75" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A75" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="75" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B75" s="5" t="s">
+      <c r="C75" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C75" s="5" t="s">
+    </row>
+    <row r="76" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A76" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B76" s="5" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="76" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B76" s="5" t="s">
+      <c r="C76" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C76" s="5" t="s">
+    </row>
+    <row r="77" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A77" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B77" s="5" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="77" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B77" s="5" t="s">
+      <c r="C77" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C77" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="78" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C78" s="5"/>
     </row>
-    <row r="79" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="79" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="4"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
     </row>
-    <row r="80" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="80" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B80" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="C80" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C80" s="5" t="s">
+    </row>
+    <row r="81" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A81" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B81" s="5" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="81" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B81" s="5" t="s">
+      <c r="C81" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C81" s="5" t="s">
+    </row>
+    <row r="82" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A82" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B82" s="5" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="82" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B82" s="5" t="s">
+      <c r="C82" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C82" s="5" t="s">
+    </row>
+    <row r="83" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A83" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B83" s="5" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="83" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B83" s="5" t="s">
+      <c r="C83" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C83" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="84" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="4"/>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
     </row>
-    <row r="85" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="85" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B85" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="C85" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C85" s="5" t="s">
+    </row>
+    <row r="86" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A86" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B86" s="5" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="86" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B86" s="5" t="s">
+      <c r="C86" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C86" s="5" t="s">
+    </row>
+    <row r="87" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A87" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B87" s="5" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="87" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B87" s="5" t="s">
+      <c r="C87" s="5"/>
+    </row>
+    <row r="88" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A88" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B88" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C87" s="5"/>
-    </row>
-    <row r="88" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>129</v>
-      </c>
       <c r="C88" s="5"/>
     </row>
-    <row r="89" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="89" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="4"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
     </row>
-    <row r="90" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="90" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B90" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="C90" s="5"/>
+    </row>
+    <row r="91" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A91" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B91" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C90" s="5"/>
-    </row>
-    <row r="91" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B91" s="5" t="s">
+      <c r="C91" s="5"/>
+    </row>
+    <row r="92" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A92" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B92" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C91" s="5"/>
-    </row>
-    <row r="92" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B92" s="5" t="s">
+      <c r="C92" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C92" s="5" t="s">
+    </row>
+    <row r="93" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A93" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B93" s="5" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="93" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B93" s="5" t="s">
+      <c r="C93" s="5"/>
+    </row>
+    <row r="94" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A94" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B94" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C93" s="5"/>
-    </row>
-    <row r="94" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B94" s="5" t="s">
+      <c r="C94" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="C94" s="5" t="s">
+    </row>
+    <row r="95" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A95" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B95" s="5" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="95" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B95" s="5" t="s">
+      <c r="C95" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C95" s="5" t="s">
+    </row>
+    <row r="96" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A96" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B96" s="5" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="96" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B96" s="5" t="s">
+      <c r="C96" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="C96" s="5" t="s">
+    </row>
+    <row r="97" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A97" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B97" s="5" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="97" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>142</v>
-      </c>
       <c r="C97" s="5"/>
     </row>
-    <row r="98" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="98" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A98" s="4"/>
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
     </row>
-    <row r="99" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="99" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A99" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B99" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B99" s="5" t="s">
+      <c r="C99" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="C99" s="5" t="s">
+    </row>
+    <row r="100" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A100" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B100" s="5" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="100" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A100" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B100" s="5" t="s">
+      <c r="C100" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C100" s="5" t="s">
+    </row>
+    <row r="101" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A101" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B101" s="5" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="101" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A101" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B101" s="5" t="s">
+      <c r="C101" s="5"/>
+    </row>
+    <row r="102" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A102" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B102" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="C101" s="5"/>
-    </row>
-    <row r="102" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B102" s="5" t="s">
+      <c r="C102" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="C102" s="5" t="s">
+    </row>
+    <row r="103" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A103" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B103" s="5" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="103" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B103" s="5" t="s">
+      <c r="C103" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="C103" s="5" t="s">
+    </row>
+    <row r="104" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A104" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B104" s="5" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="104" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A104" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B104" s="5" t="s">
+      <c r="C104" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C104" s="5" t="s">
+    </row>
+    <row r="105" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A105" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B105" s="5" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="105" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B105" s="5" t="s">
+      <c r="C105" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C105" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="106" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A106" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C106" s="5"/>
     </row>
-    <row r="107" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="107" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A107" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B107" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C107" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C107" s="5" t="s">
+    </row>
+    <row r="108" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A108" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B108" s="5" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="108" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B108" s="5" t="s">
+      <c r="C108" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C108" s="5" t="s">
+    </row>
+    <row r="109" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A109" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B109" s="5" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="109" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B109" s="5" t="s">
+      <c r="C109" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="C109" s="5" t="s">
-        <v>162</v>
-      </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="1" right="1" top="1" bottom="1" header="0.511805555555555" footer="0.25"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddFooter>&amp;C&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>

</xml_diff>